<commit_message>
new candidates update + new colors + change of order of coalitions
</commit_message>
<xml_diff>
--- a/diccionario_coalicion.xlsx
+++ b/diccionario_coalicion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goyan\Desktop\bc-aut\bc-autonomo-mapas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D1500D-B856-4EB1-B69D-1C6006EF5AB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04A086D-F2ED-4906-9C87-6CAEAAFEE5E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="78">
   <si>
     <t>Independientes de Tarapacá</t>
   </si>
@@ -594,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B74"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1198,6 +1198,30 @@
         <v>1</v>
       </c>
     </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>